<commit_message>
Update show name english only.
</commit_message>
<xml_diff>
--- a/form/Product/price_list.xlsx
+++ b/form/Product/price_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AppServ\www\erp_mvc\form\Product\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4374EDA5-0B4A-4F29-ADDA-269BA26710FC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C995239F-7589-48DD-9447-851419F6B889}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{86297DB4-77BC-4104-933B-EBA1FFAEFF5A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>103-75100L</t>
   </si>
@@ -85,9 +85,6 @@
   </si>
   <si>
     <t>103-75100Lg</t>
-  </si>
-  <si>
-    <t>WNDC/1-16-88/BT40</t>
   </si>
   <si>
     <t>MRGN400-A-H01</t>
@@ -100,7 +97,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,6 +119,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -171,7 +174,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -188,6 +191,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4C0EC3C-8197-4F9F-A4D9-C6E0490B4AA3}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="19.899999999999999" customHeight="1"/>
@@ -848,8 +852,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="19.899999999999999" customHeight="1">
-      <c r="A15" s="4" t="s">
-        <v>20</v>
+      <c r="A15" s="8">
+        <v>104136</v>
       </c>
       <c r="B15" s="2">
         <v>2500</v>
@@ -873,7 +877,7 @@
     </row>
     <row r="16" spans="1:6" ht="19.899999999999999" customHeight="1">
       <c r="A16" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" s="2">
         <v>1236</v>
@@ -897,7 +901,7 @@
     </row>
     <row r="17" spans="1:6" ht="19.899999999999999" customHeight="1">
       <c r="A17" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" s="2">
         <v>256</v>

</xml_diff>